<commit_message>
dados prateleira 2 inseridos
</commit_message>
<xml_diff>
--- a/banco/grupo3.xlsx
+++ b/banco/grupo3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="292">
   <si>
     <t>Classe</t>
   </si>
@@ -263,6 +263,81 @@
     <t>75</t>
   </si>
   <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
     <t>Classe 2</t>
   </si>
   <si>
@@ -341,6 +416,81 @@
     <t>19(430) H333p =60</t>
   </si>
   <si>
+    <t>23(09) H289L</t>
+  </si>
+  <si>
+    <t>233 B496r =60</t>
+  </si>
+  <si>
+    <t>241 C482a</t>
+  </si>
+  <si>
+    <t>244 C434L</t>
+  </si>
+  <si>
+    <t>245 C231p</t>
+  </si>
+  <si>
+    <t>248 L929s</t>
+  </si>
+  <si>
+    <t>261.6 A239h =690</t>
+  </si>
+  <si>
+    <t>261.6 A447i</t>
+  </si>
+  <si>
+    <t>271.5(81)(09) L533h</t>
+  </si>
+  <si>
+    <t>266.5 D547n</t>
+  </si>
+  <si>
+    <t>266(7/8)(09) S759e</t>
+  </si>
+  <si>
+    <t>264 B782L</t>
+  </si>
+  <si>
+    <t>261.7 (469) N778i</t>
+  </si>
+  <si>
+    <t>248.153.6 L929s =690</t>
+  </si>
+  <si>
+    <t>248.1 A983v</t>
+  </si>
+  <si>
+    <t>241:282 F951m =690</t>
+  </si>
+  <si>
+    <t>241 G791t</t>
+  </si>
+  <si>
+    <t>234.1 F382k</t>
+  </si>
+  <si>
+    <t>230 C928c</t>
+  </si>
+  <si>
+    <t>226.4 C147d</t>
+  </si>
+  <si>
+    <t>221 R832cL =60</t>
+  </si>
+  <si>
+    <t>229.8 A643p</t>
+  </si>
+  <si>
+    <t>231 B536d</t>
+  </si>
+  <si>
+    <t>232.9 B673j</t>
+  </si>
+  <si>
+    <t>232.9 H542m =690</t>
+  </si>
+  <si>
     <t>297.18 =20 A354q</t>
   </si>
   <si>
@@ -491,9 +641,6 @@
     <t>299.992 L617r =690</t>
   </si>
   <si>
-    <t>90</t>
-  </si>
-  <si>
     <t>239</t>
   </si>
   <si>
@@ -557,7 +704,73 @@
     <t>1147</t>
   </si>
   <si>
-    <t>93</t>
+    <t>141</t>
+  </si>
+  <si>
+    <t>198</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>332</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>538</t>
+  </si>
+  <si>
+    <t>581</t>
+  </si>
+  <si>
+    <t>614</t>
+  </si>
+  <si>
+    <t>628</t>
+  </si>
+  <si>
+    <t>682</t>
+  </si>
+  <si>
+    <t>801</t>
+  </si>
+  <si>
+    <t>836</t>
+  </si>
+  <si>
+    <t>854</t>
+  </si>
+  <si>
+    <t>886</t>
+  </si>
+  <si>
+    <t>996</t>
+  </si>
+  <si>
+    <t>1047</t>
+  </si>
+  <si>
+    <t>1069</t>
+  </si>
+  <si>
+    <t>1127</t>
+  </si>
+  <si>
+    <t>1160</t>
+  </si>
+  <si>
+    <t>1181</t>
+  </si>
+  <si>
+    <t>1197</t>
   </si>
   <si>
     <t>112</t>
@@ -627,18 +840,6 @@
   </si>
   <si>
     <t>1245</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>100</t>
   </si>
   <si>
     <t>103</t>
@@ -769,19 +970,19 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F2" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G2" t="e">
         <v>#N/A</v>
@@ -798,19 +999,19 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F3" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G3" t="e">
         <v>#N/A</v>
@@ -827,19 +1028,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
         <v>81</v>
       </c>
       <c r="E4" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F4" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G4" t="e">
         <v>#N/A</v>
@@ -856,13 +1057,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -874,7 +1075,7 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>222</v>
+        <v>289</v>
       </c>
       <c r="I5" t="s">
         <v>8</v>
@@ -885,13 +1086,13 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -903,7 +1104,7 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>222</v>
+        <v>289</v>
       </c>
       <c r="I6" t="s">
         <v>8</v>
@@ -914,13 +1115,13 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>210</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -932,7 +1133,7 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>222</v>
+        <v>289</v>
       </c>
       <c r="I7" t="s">
         <v>8</v>
@@ -943,13 +1144,13 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -961,7 +1162,7 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>222</v>
+        <v>289</v>
       </c>
       <c r="I8" t="s">
         <v>8</v>
@@ -972,13 +1173,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -990,7 +1191,7 @@
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>222</v>
+        <v>289</v>
       </c>
       <c r="I9" t="s">
         <v>8</v>
@@ -1001,13 +1202,13 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>213</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1019,7 +1220,7 @@
         <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I10" t="s">
         <v>8</v>
@@ -1030,19 +1231,19 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="E11" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F11" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G11" t="e">
         <v>#N/A</v>
@@ -1059,13 +1260,13 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>215</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -1077,7 +1278,7 @@
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I12" t="s">
         <v>8</v>
@@ -1088,13 +1289,13 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>216</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1106,7 +1307,7 @@
         <v>9</v>
       </c>
       <c r="H13" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I13" t="s">
         <v>8</v>
@@ -1117,13 +1318,13 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="D14" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1135,7 +1336,7 @@
         <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I14" t="s">
         <v>8</v>
@@ -1146,13 +1347,13 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>218</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1164,7 +1365,7 @@
         <v>9</v>
       </c>
       <c r="H15" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I15" t="s">
         <v>8</v>
@@ -1175,13 +1376,13 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1193,7 +1394,7 @@
         <v>9</v>
       </c>
       <c r="H16" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I16" t="s">
         <v>8</v>
@@ -1204,19 +1405,19 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="D17" t="s">
-        <v>171</v>
+        <v>220</v>
       </c>
       <c r="E17" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F17" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G17" t="e">
         <v>#N/A</v>
@@ -1233,19 +1434,19 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>172</v>
+        <v>221</v>
       </c>
       <c r="E18" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F18" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G18" t="e">
         <v>#N/A</v>
@@ -1262,13 +1463,13 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>222</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1280,7 +1481,7 @@
         <v>9</v>
       </c>
       <c r="H19" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I19" t="s">
         <v>8</v>
@@ -1291,13 +1492,13 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="D20" t="s">
-        <v>174</v>
+        <v>223</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -1309,7 +1510,7 @@
         <v>9</v>
       </c>
       <c r="H20" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I20" t="s">
         <v>8</v>
@@ -1320,13 +1521,13 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1338,7 +1539,7 @@
         <v>9</v>
       </c>
       <c r="H21" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I21" t="s">
         <v>8</v>
@@ -1349,19 +1550,19 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>225</v>
       </c>
       <c r="E22" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F22" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G22" t="e">
         <v>#N/A</v>
@@ -1378,19 +1579,19 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
       <c r="E23" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F23" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G23" t="e">
         <v>#N/A</v>
@@ -1407,13 +1608,13 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1425,7 +1626,7 @@
         <v>9</v>
       </c>
       <c r="H24" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I24" t="s">
         <v>8</v>
@@ -1436,13 +1637,13 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>228</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1454,7 +1655,7 @@
         <v>10</v>
       </c>
       <c r="H25" t="s">
-        <v>222</v>
+        <v>289</v>
       </c>
       <c r="I25" t="s">
         <v>8</v>
@@ -1465,19 +1666,19 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="D26" t="s">
-        <v>180</v>
+        <v>229</v>
       </c>
       <c r="E26" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F26" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G26" t="e">
         <v>#N/A</v>
@@ -1494,13 +1695,13 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1509,13 +1710,13 @@
         <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>223</v>
+        <v>291</v>
       </c>
       <c r="I27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28">
@@ -1523,28 +1724,28 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="D28" t="s">
-        <v>181</v>
+        <v>230</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F28" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" t="s">
-        <v>222</v>
+        <v>288</v>
+      </c>
+      <c r="G28" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H28" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29">
@@ -1552,28 +1753,28 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="D29" t="s">
-        <v>182</v>
+        <v>231</v>
       </c>
       <c r="E29" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>221</v>
-      </c>
-      <c r="G29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H29" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" t="s">
+        <v>291</v>
       </c>
       <c r="I29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
@@ -1581,28 +1782,28 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="D30" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
       <c r="E30" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>221</v>
-      </c>
-      <c r="G30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H30" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G30" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" t="s">
+        <v>290</v>
       </c>
       <c r="I30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31">
@@ -1610,28 +1811,28 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="D31" t="s">
-        <v>184</v>
+        <v>233</v>
       </c>
       <c r="E31" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>221</v>
-      </c>
-      <c r="G31" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H31" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" t="s">
+        <v>291</v>
       </c>
       <c r="I31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
@@ -1639,28 +1840,28 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="E32" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>221</v>
-      </c>
-      <c r="G32" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H32" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>291</v>
       </c>
       <c r="I32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33">
@@ -1668,28 +1869,28 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="D33" t="s">
-        <v>186</v>
+        <v>235</v>
       </c>
       <c r="E33" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
-        <v>221</v>
-      </c>
-      <c r="G33" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H33" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" t="s">
+        <v>291</v>
       </c>
       <c r="I33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34">
@@ -1697,19 +1898,19 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="D34" t="s">
-        <v>187</v>
+        <v>236</v>
       </c>
       <c r="E34" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F34" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G34" t="e">
         <v>#N/A</v>
@@ -1718,7 +1919,7 @@
         <v>#N/A</v>
       </c>
       <c r="I34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35">
@@ -1726,28 +1927,28 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
       <c r="D35" t="s">
-        <v>188</v>
+        <v>237</v>
       </c>
       <c r="E35" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F35" t="s">
-        <v>221</v>
-      </c>
-      <c r="G35" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H35" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" t="s">
+        <v>291</v>
       </c>
       <c r="I35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36">
@@ -1755,28 +1956,28 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="D36" t="s">
-        <v>189</v>
+        <v>238</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F36" t="s">
-        <v>3</v>
-      </c>
-      <c r="G36" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" t="s">
-        <v>223</v>
+        <v>288</v>
+      </c>
+      <c r="G36" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H36" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37">
@@ -1784,19 +1985,19 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="D37" t="s">
-        <v>190</v>
+        <v>239</v>
       </c>
       <c r="E37" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F37" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G37" t="e">
         <v>#N/A</v>
@@ -1805,7 +2006,7 @@
         <v>#N/A</v>
       </c>
       <c r="I37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
@@ -1813,28 +2014,28 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="D38" t="s">
-        <v>191</v>
+        <v>240</v>
       </c>
       <c r="E38" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F38" t="s">
-        <v>221</v>
-      </c>
-      <c r="G38" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H38" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>10</v>
+      </c>
+      <c r="H38" t="s">
+        <v>289</v>
       </c>
       <c r="I38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
@@ -1842,28 +2043,28 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="E39" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
-        <v>221</v>
-      </c>
-      <c r="G39" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H39" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" t="s">
+        <v>291</v>
       </c>
       <c r="I39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
@@ -1871,19 +2072,19 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="D40" t="s">
-        <v>193</v>
+        <v>242</v>
       </c>
       <c r="E40" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F40" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G40" t="e">
         <v>#N/A</v>
@@ -1892,7 +2093,7 @@
         <v>#N/A</v>
       </c>
       <c r="I40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41">
@@ -1900,19 +2101,19 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="D41" t="s">
-        <v>194</v>
+        <v>243</v>
       </c>
       <c r="E41" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F41" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G41" t="e">
         <v>#N/A</v>
@@ -1921,7 +2122,7 @@
         <v>#N/A</v>
       </c>
       <c r="I41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42">
@@ -1929,28 +2130,28 @@
         <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="D42" t="s">
-        <v>195</v>
+        <v>244</v>
       </c>
       <c r="E42" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>221</v>
-      </c>
-      <c r="G42" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H42" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" t="s">
+        <v>291</v>
       </c>
       <c r="I42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
@@ -1958,28 +2159,28 @@
         <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="D43" t="s">
-        <v>196</v>
+        <v>245</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F43" t="s">
-        <v>3</v>
-      </c>
-      <c r="G43" t="s">
-        <v>10</v>
-      </c>
-      <c r="H43" t="s">
-        <v>222</v>
+        <v>288</v>
+      </c>
+      <c r="G43" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H43" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44">
@@ -1987,28 +2188,28 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="D44" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="E44" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>221</v>
-      </c>
-      <c r="G44" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H44" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" t="s">
+        <v>290</v>
       </c>
       <c r="I44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45">
@@ -2016,28 +2217,28 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="D45" t="s">
-        <v>198</v>
+        <v>246</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G45" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" t="s">
-        <v>222</v>
+        <v>288</v>
+      </c>
+      <c r="G45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H45" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46">
@@ -2045,19 +2246,19 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>247</v>
       </c>
       <c r="E46" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F46" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G46" t="e">
         <v>#N/A</v>
@@ -2066,7 +2267,7 @@
         <v>#N/A</v>
       </c>
       <c r="I46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47">
@@ -2074,19 +2275,19 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="D47" t="s">
-        <v>200</v>
+        <v>248</v>
       </c>
       <c r="E47" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F47" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G47" t="e">
         <v>#N/A</v>
@@ -2095,7 +2296,7 @@
         <v>#N/A</v>
       </c>
       <c r="I47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48">
@@ -2103,28 +2304,28 @@
         <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D48" t="s">
-        <v>201</v>
+        <v>249</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F48" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48" t="s">
-        <v>223</v>
+        <v>288</v>
+      </c>
+      <c r="G48" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H48" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49">
@@ -2132,19 +2333,19 @@
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>250</v>
       </c>
       <c r="E49" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F49" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G49" t="e">
         <v>#N/A</v>
@@ -2153,7 +2354,7 @@
         <v>#N/A</v>
       </c>
       <c r="I49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50">
@@ -2161,13 +2362,13 @@
         <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="D50" t="s">
-        <v>203</v>
+        <v>251</v>
       </c>
       <c r="E50" t="s">
         <v>8</v>
@@ -2179,10 +2380,10 @@
         <v>8</v>
       </c>
       <c r="H50" t="s">
-        <v>224</v>
+        <v>291</v>
       </c>
       <c r="I50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51">
@@ -2190,28 +2391,28 @@
         <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="D51" t="s">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="E51" t="s">
-        <v>220</v>
+        <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>221</v>
-      </c>
-      <c r="G51" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H51" t="e">
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="G51" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" t="s">
+        <v>291</v>
       </c>
       <c r="I51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52">
@@ -2219,13 +2420,13 @@
         <v>58</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
@@ -2237,10 +2438,10 @@
         <v>9</v>
       </c>
       <c r="H52" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53">
@@ -2248,13 +2449,13 @@
         <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
@@ -2263,13 +2464,13 @@
         <v>3</v>
       </c>
       <c r="G53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H53" t="s">
-        <v>223</v>
+        <v>289</v>
       </c>
       <c r="I53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54">
@@ -2277,28 +2478,28 @@
         <v>60</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="D54" t="s">
-        <v>34</v>
+        <v>253</v>
       </c>
       <c r="E54" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F54" t="s">
-        <v>3</v>
-      </c>
-      <c r="G54" t="s">
-        <v>8</v>
-      </c>
-      <c r="H54" t="s">
-        <v>224</v>
+        <v>288</v>
+      </c>
+      <c r="G54" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H54" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55">
@@ -2306,28 +2507,28 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>37</v>
+        <v>254</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F55" t="s">
-        <v>3</v>
-      </c>
-      <c r="G55" t="s">
-        <v>9</v>
-      </c>
-      <c r="H55" t="s">
-        <v>223</v>
+        <v>288</v>
+      </c>
+      <c r="G55" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H55" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56">
@@ -2335,28 +2536,28 @@
         <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="D56" t="s">
-        <v>49</v>
+        <v>255</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F56" t="s">
-        <v>3</v>
-      </c>
-      <c r="G56" t="s">
-        <v>10</v>
-      </c>
-      <c r="H56" t="s">
-        <v>222</v>
+        <v>288</v>
+      </c>
+      <c r="G56" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H56" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57">
@@ -2364,19 +2565,19 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C57" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="D57" t="s">
-        <v>58</v>
+        <v>256</v>
       </c>
       <c r="E57" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F57" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G57" t="e">
         <v>#N/A</v>
@@ -2385,7 +2586,7 @@
         <v>#N/A</v>
       </c>
       <c r="I57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58">
@@ -2393,19 +2594,19 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="D58" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="E58" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F58" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G58" t="e">
         <v>#N/A</v>
@@ -2414,7 +2615,7 @@
         <v>#N/A</v>
       </c>
       <c r="I58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59">
@@ -2422,19 +2623,19 @@
         <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C59" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="D59" t="s">
-        <v>70</v>
+        <v>258</v>
       </c>
       <c r="E59" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F59" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G59" t="e">
         <v>#N/A</v>
@@ -2443,7 +2644,7 @@
         <v>#N/A</v>
       </c>
       <c r="I59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60">
@@ -2451,28 +2652,28 @@
         <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C60" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="D60" t="s">
-        <v>77</v>
+        <v>259</v>
       </c>
       <c r="E60" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F60" t="s">
-        <v>3</v>
-      </c>
-      <c r="G60" t="s">
-        <v>9</v>
-      </c>
-      <c r="H60" t="s">
-        <v>223</v>
+        <v>288</v>
+      </c>
+      <c r="G60" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H60" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61">
@@ -2480,13 +2681,13 @@
         <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C61" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="D61" t="s">
-        <v>79</v>
+        <v>260</v>
       </c>
       <c r="E61" t="s">
         <v>8</v>
@@ -2498,10 +2699,10 @@
         <v>9</v>
       </c>
       <c r="H61" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62">
@@ -2509,28 +2710,28 @@
         <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C62" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="D62" t="s">
-        <v>205</v>
+        <v>261</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F62" t="s">
-        <v>3</v>
-      </c>
-      <c r="G62" t="s">
-        <v>8</v>
-      </c>
-      <c r="H62" t="s">
-        <v>224</v>
+        <v>288</v>
+      </c>
+      <c r="G62" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H62" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63">
@@ -2538,19 +2739,19 @@
         <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="D63" t="s">
-        <v>206</v>
+        <v>262</v>
       </c>
       <c r="E63" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F63" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G63" t="e">
         <v>#N/A</v>
@@ -2559,7 +2760,7 @@
         <v>#N/A</v>
       </c>
       <c r="I63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64">
@@ -2567,19 +2768,19 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>207</v>
+        <v>263</v>
       </c>
       <c r="E64" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F64" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G64" t="e">
         <v>#N/A</v>
@@ -2588,7 +2789,7 @@
         <v>#N/A</v>
       </c>
       <c r="I64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65">
@@ -2596,28 +2797,28 @@
         <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C65" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="D65" t="s">
-        <v>208</v>
+        <v>264</v>
       </c>
       <c r="E65" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F65" t="s">
-        <v>3</v>
-      </c>
-      <c r="G65" t="s">
-        <v>9</v>
-      </c>
-      <c r="H65" t="s">
-        <v>223</v>
+        <v>288</v>
+      </c>
+      <c r="G65" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H65" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66">
@@ -2625,28 +2826,28 @@
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="D66" t="s">
-        <v>209</v>
+        <v>265</v>
       </c>
       <c r="E66" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F66" t="s">
-        <v>3</v>
-      </c>
-      <c r="G66" t="s">
-        <v>9</v>
-      </c>
-      <c r="H66" t="s">
-        <v>223</v>
+        <v>288</v>
+      </c>
+      <c r="G66" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H66" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67">
@@ -2654,19 +2855,19 @@
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="D67" t="s">
-        <v>210</v>
+        <v>266</v>
       </c>
       <c r="E67" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
       <c r="F67" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="G67" t="e">
         <v>#N/A</v>
@@ -2675,7 +2876,7 @@
         <v>#N/A</v>
       </c>
       <c r="I67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68">
@@ -2683,13 +2884,13 @@
         <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="D68" t="s">
-        <v>211</v>
+        <v>267</v>
       </c>
       <c r="E68" t="s">
         <v>8</v>
@@ -2698,13 +2899,13 @@
         <v>3</v>
       </c>
       <c r="G68" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H68" t="s">
-        <v>223</v>
+        <v>289</v>
       </c>
       <c r="I68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69">
@@ -2712,28 +2913,28 @@
         <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="D69" t="s">
-        <v>212</v>
+        <v>268</v>
       </c>
       <c r="E69" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F69" t="s">
-        <v>3</v>
-      </c>
-      <c r="G69" t="s">
-        <v>10</v>
-      </c>
-      <c r="H69" t="s">
-        <v>222</v>
+        <v>288</v>
+      </c>
+      <c r="G69" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H69" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70">
@@ -2741,13 +2942,13 @@
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C70" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="D70" t="s">
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="E70" t="s">
         <v>8</v>
@@ -2756,13 +2957,13 @@
         <v>3</v>
       </c>
       <c r="G70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H70" t="s">
-        <v>223</v>
+        <v>289</v>
       </c>
       <c r="I70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71">
@@ -2770,28 +2971,28 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C71" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="D71" t="s">
-        <v>214</v>
+        <v>270</v>
       </c>
       <c r="E71" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F71" t="s">
-        <v>3</v>
-      </c>
-      <c r="G71" t="s">
-        <v>10</v>
-      </c>
-      <c r="H71" t="s">
-        <v>222</v>
+        <v>288</v>
+      </c>
+      <c r="G71" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H71" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72">
@@ -2799,28 +3000,28 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C72" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="D72" t="s">
-        <v>215</v>
+        <v>271</v>
       </c>
       <c r="E72" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F72" t="s">
-        <v>3</v>
-      </c>
-      <c r="G72" t="s">
-        <v>9</v>
-      </c>
-      <c r="H72" t="s">
-        <v>223</v>
+        <v>288</v>
+      </c>
+      <c r="G72" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H72" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73">
@@ -2828,13 +3029,13 @@
         <v>79</v>
       </c>
       <c r="B73" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C73" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="D73" t="s">
-        <v>216</v>
+        <v>272</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
@@ -2846,10 +3047,10 @@
         <v>9</v>
       </c>
       <c r="H73" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="I73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74">
@@ -2857,28 +3058,28 @@
         <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C74" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="D74" t="s">
-        <v>217</v>
+        <v>273</v>
       </c>
       <c r="E74" t="s">
-        <v>8</v>
+        <v>287</v>
       </c>
       <c r="F74" t="s">
-        <v>3</v>
-      </c>
-      <c r="G74" t="s">
-        <v>10</v>
-      </c>
-      <c r="H74" t="s">
-        <v>222</v>
+        <v>288</v>
+      </c>
+      <c r="G74" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H74" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75">
@@ -2886,13 +3087,13 @@
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C75" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="D75" t="s">
-        <v>218</v>
+        <v>274</v>
       </c>
       <c r="E75" t="s">
         <v>8</v>
@@ -2901,13 +3102,13 @@
         <v>3</v>
       </c>
       <c r="G75" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H75" t="s">
-        <v>223</v>
+        <v>291</v>
       </c>
       <c r="I75" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76">
@@ -2915,27 +3116,752 @@
         <v>82</v>
       </c>
       <c r="B76" t="s">
+        <v>108</v>
+      </c>
+      <c r="C76" t="s">
+        <v>183</v>
+      </c>
+      <c r="D76" t="s">
+        <v>275</v>
+      </c>
+      <c r="E76" t="s">
+        <v>287</v>
+      </c>
+      <c r="F76" t="s">
+        <v>288</v>
+      </c>
+      <c r="G76" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H76" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I76" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
         <v>83</v>
       </c>
-      <c r="C76" t="s">
-        <v>158</v>
-      </c>
-      <c r="D76" t="s">
-        <v>219</v>
-      </c>
-      <c r="E76" t="s">
-        <v>8</v>
-      </c>
-      <c r="F76" t="s">
-        <v>3</v>
-      </c>
-      <c r="G76" t="s">
-        <v>10</v>
-      </c>
-      <c r="H76" t="s">
-        <v>222</v>
-      </c>
-      <c r="I76" t="s">
+      <c r="B77" t="s">
+        <v>108</v>
+      </c>
+      <c r="C77" t="s">
+        <v>184</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" t="s">
+        <v>3</v>
+      </c>
+      <c r="G77" t="s">
+        <v>9</v>
+      </c>
+      <c r="H77" t="s">
+        <v>290</v>
+      </c>
+      <c r="I77" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>84</v>
+      </c>
+      <c r="B78" t="s">
+        <v>108</v>
+      </c>
+      <c r="C78" t="s">
+        <v>185</v>
+      </c>
+      <c r="D78" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" t="s">
+        <v>3</v>
+      </c>
+      <c r="G78" t="s">
+        <v>9</v>
+      </c>
+      <c r="H78" t="s">
+        <v>290</v>
+      </c>
+      <c r="I78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" t="s">
+        <v>108</v>
+      </c>
+      <c r="C79" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79" t="s">
+        <v>34</v>
+      </c>
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" t="s">
+        <v>3</v>
+      </c>
+      <c r="G79" t="s">
+        <v>8</v>
+      </c>
+      <c r="H79" t="s">
+        <v>291</v>
+      </c>
+      <c r="I79" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" t="s">
+        <v>108</v>
+      </c>
+      <c r="C80" t="s">
+        <v>187</v>
+      </c>
+      <c r="D80" t="s">
+        <v>37</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" t="s">
+        <v>3</v>
+      </c>
+      <c r="G80" t="s">
+        <v>9</v>
+      </c>
+      <c r="H80" t="s">
+        <v>290</v>
+      </c>
+      <c r="I80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>87</v>
+      </c>
+      <c r="B81" t="s">
+        <v>108</v>
+      </c>
+      <c r="C81" t="s">
+        <v>188</v>
+      </c>
+      <c r="D81" t="s">
+        <v>49</v>
+      </c>
+      <c r="E81" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" t="s">
+        <v>3</v>
+      </c>
+      <c r="G81" t="s">
+        <v>10</v>
+      </c>
+      <c r="H81" t="s">
+        <v>289</v>
+      </c>
+      <c r="I81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>88</v>
+      </c>
+      <c r="B82" t="s">
+        <v>108</v>
+      </c>
+      <c r="C82" t="s">
+        <v>189</v>
+      </c>
+      <c r="D82" t="s">
+        <v>58</v>
+      </c>
+      <c r="E82" t="s">
+        <v>287</v>
+      </c>
+      <c r="F82" t="s">
+        <v>288</v>
+      </c>
+      <c r="G82" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H82" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I82" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>89</v>
+      </c>
+      <c r="B83" t="s">
+        <v>108</v>
+      </c>
+      <c r="C83" t="s">
+        <v>190</v>
+      </c>
+      <c r="D83" t="s">
+        <v>63</v>
+      </c>
+      <c r="E83" t="s">
+        <v>287</v>
+      </c>
+      <c r="F83" t="s">
+        <v>288</v>
+      </c>
+      <c r="G83" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H83" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I83" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B84" t="s">
+        <v>108</v>
+      </c>
+      <c r="C84" t="s">
+        <v>191</v>
+      </c>
+      <c r="D84" t="s">
+        <v>70</v>
+      </c>
+      <c r="E84" t="s">
+        <v>287</v>
+      </c>
+      <c r="F84" t="s">
+        <v>288</v>
+      </c>
+      <c r="G84" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H84" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85" t="s">
+        <v>108</v>
+      </c>
+      <c r="C85" t="s">
+        <v>192</v>
+      </c>
+      <c r="D85" t="s">
+        <v>77</v>
+      </c>
+      <c r="E85" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" t="s">
+        <v>3</v>
+      </c>
+      <c r="G85" t="s">
+        <v>9</v>
+      </c>
+      <c r="H85" t="s">
+        <v>290</v>
+      </c>
+      <c r="I85" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>92</v>
+      </c>
+      <c r="B86" t="s">
+        <v>108</v>
+      </c>
+      <c r="C86" t="s">
+        <v>193</v>
+      </c>
+      <c r="D86" t="s">
+        <v>79</v>
+      </c>
+      <c r="E86" t="s">
+        <v>8</v>
+      </c>
+      <c r="F86" t="s">
+        <v>3</v>
+      </c>
+      <c r="G86" t="s">
+        <v>9</v>
+      </c>
+      <c r="H86" t="s">
+        <v>290</v>
+      </c>
+      <c r="I86" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>93</v>
+      </c>
+      <c r="B87" t="s">
+        <v>108</v>
+      </c>
+      <c r="C87" t="s">
+        <v>194</v>
+      </c>
+      <c r="D87" t="s">
+        <v>86</v>
+      </c>
+      <c r="E87" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" t="s">
+        <v>3</v>
+      </c>
+      <c r="G87" t="s">
+        <v>8</v>
+      </c>
+      <c r="H87" t="s">
+        <v>291</v>
+      </c>
+      <c r="I87" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>94</v>
+      </c>
+      <c r="B88" t="s">
+        <v>108</v>
+      </c>
+      <c r="C88" t="s">
+        <v>195</v>
+      </c>
+      <c r="D88" t="s">
+        <v>87</v>
+      </c>
+      <c r="E88" t="s">
+        <v>287</v>
+      </c>
+      <c r="F88" t="s">
+        <v>288</v>
+      </c>
+      <c r="G88" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H88" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I88" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>95</v>
+      </c>
+      <c r="B89" t="s">
+        <v>108</v>
+      </c>
+      <c r="C89" t="s">
+        <v>196</v>
+      </c>
+      <c r="D89" t="s">
+        <v>102</v>
+      </c>
+      <c r="E89" t="s">
+        <v>287</v>
+      </c>
+      <c r="F89" t="s">
+        <v>288</v>
+      </c>
+      <c r="G89" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H89" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I89" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>96</v>
+      </c>
+      <c r="B90" t="s">
+        <v>108</v>
+      </c>
+      <c r="C90" t="s">
+        <v>197</v>
+      </c>
+      <c r="D90" t="s">
+        <v>107</v>
+      </c>
+      <c r="E90" t="s">
+        <v>8</v>
+      </c>
+      <c r="F90" t="s">
+        <v>3</v>
+      </c>
+      <c r="G90" t="s">
+        <v>9</v>
+      </c>
+      <c r="H90" t="s">
+        <v>290</v>
+      </c>
+      <c r="I90" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>97</v>
+      </c>
+      <c r="B91" t="s">
+        <v>108</v>
+      </c>
+      <c r="C91" t="s">
+        <v>198</v>
+      </c>
+      <c r="D91" t="s">
+        <v>276</v>
+      </c>
+      <c r="E91" t="s">
+        <v>8</v>
+      </c>
+      <c r="F91" t="s">
+        <v>3</v>
+      </c>
+      <c r="G91" t="s">
+        <v>9</v>
+      </c>
+      <c r="H91" t="s">
+        <v>290</v>
+      </c>
+      <c r="I91" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>98</v>
+      </c>
+      <c r="B92" t="s">
+        <v>108</v>
+      </c>
+      <c r="C92" t="s">
+        <v>199</v>
+      </c>
+      <c r="D92" t="s">
+        <v>277</v>
+      </c>
+      <c r="E92" t="s">
+        <v>287</v>
+      </c>
+      <c r="F92" t="s">
+        <v>288</v>
+      </c>
+      <c r="G92" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H92" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I92" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>99</v>
+      </c>
+      <c r="B93" t="s">
+        <v>108</v>
+      </c>
+      <c r="C93" t="s">
+        <v>200</v>
+      </c>
+      <c r="D93" t="s">
+        <v>278</v>
+      </c>
+      <c r="E93" t="s">
+        <v>8</v>
+      </c>
+      <c r="F93" t="s">
+        <v>3</v>
+      </c>
+      <c r="G93" t="s">
+        <v>9</v>
+      </c>
+      <c r="H93" t="s">
+        <v>290</v>
+      </c>
+      <c r="I93" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>100</v>
+      </c>
+      <c r="B94" t="s">
+        <v>108</v>
+      </c>
+      <c r="C94" t="s">
+        <v>201</v>
+      </c>
+      <c r="D94" t="s">
+        <v>279</v>
+      </c>
+      <c r="E94" t="s">
+        <v>8</v>
+      </c>
+      <c r="F94" t="s">
+        <v>3</v>
+      </c>
+      <c r="G94" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" t="s">
+        <v>289</v>
+      </c>
+      <c r="I94" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>101</v>
+      </c>
+      <c r="B95" t="s">
+        <v>108</v>
+      </c>
+      <c r="C95" t="s">
+        <v>202</v>
+      </c>
+      <c r="D95" t="s">
+        <v>280</v>
+      </c>
+      <c r="E95" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" t="s">
+        <v>3</v>
+      </c>
+      <c r="G95" t="s">
+        <v>9</v>
+      </c>
+      <c r="H95" t="s">
+        <v>290</v>
+      </c>
+      <c r="I95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>102</v>
+      </c>
+      <c r="B96" t="s">
+        <v>108</v>
+      </c>
+      <c r="C96" t="s">
+        <v>203</v>
+      </c>
+      <c r="D96" t="s">
+        <v>281</v>
+      </c>
+      <c r="E96" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" t="s">
+        <v>3</v>
+      </c>
+      <c r="G96" t="s">
+        <v>10</v>
+      </c>
+      <c r="H96" t="s">
+        <v>289</v>
+      </c>
+      <c r="I96" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>103</v>
+      </c>
+      <c r="B97" t="s">
+        <v>108</v>
+      </c>
+      <c r="C97" t="s">
+        <v>204</v>
+      </c>
+      <c r="D97" t="s">
+        <v>282</v>
+      </c>
+      <c r="E97" t="s">
+        <v>8</v>
+      </c>
+      <c r="F97" t="s">
+        <v>3</v>
+      </c>
+      <c r="G97" t="s">
+        <v>9</v>
+      </c>
+      <c r="H97" t="s">
+        <v>290</v>
+      </c>
+      <c r="I97" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>104</v>
+      </c>
+      <c r="B98" t="s">
+        <v>108</v>
+      </c>
+      <c r="C98" t="s">
+        <v>205</v>
+      </c>
+      <c r="D98" t="s">
+        <v>283</v>
+      </c>
+      <c r="E98" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98" t="s">
+        <v>3</v>
+      </c>
+      <c r="G98" t="s">
+        <v>9</v>
+      </c>
+      <c r="H98" t="s">
+        <v>290</v>
+      </c>
+      <c r="I98" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>105</v>
+      </c>
+      <c r="B99" t="s">
+        <v>108</v>
+      </c>
+      <c r="C99" t="s">
+        <v>206</v>
+      </c>
+      <c r="D99" t="s">
+        <v>284</v>
+      </c>
+      <c r="E99" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" t="s">
+        <v>3</v>
+      </c>
+      <c r="G99" t="s">
+        <v>10</v>
+      </c>
+      <c r="H99" t="s">
+        <v>289</v>
+      </c>
+      <c r="I99" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>106</v>
+      </c>
+      <c r="B100" t="s">
+        <v>108</v>
+      </c>
+      <c r="C100" t="s">
+        <v>207</v>
+      </c>
+      <c r="D100" t="s">
+        <v>285</v>
+      </c>
+      <c r="E100" t="s">
+        <v>8</v>
+      </c>
+      <c r="F100" t="s">
+        <v>3</v>
+      </c>
+      <c r="G100" t="s">
+        <v>9</v>
+      </c>
+      <c r="H100" t="s">
+        <v>290</v>
+      </c>
+      <c r="I100" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>107</v>
+      </c>
+      <c r="B101" t="s">
+        <v>108</v>
+      </c>
+      <c r="C101" t="s">
+        <v>208</v>
+      </c>
+      <c r="D101" t="s">
+        <v>286</v>
+      </c>
+      <c r="E101" t="s">
+        <v>8</v>
+      </c>
+      <c r="F101" t="s">
+        <v>3</v>
+      </c>
+      <c r="G101" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" t="s">
+        <v>289</v>
+      </c>
+      <c r="I101" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>